<commit_message>
sales & redemp report
</commit_message>
<xml_diff>
--- a/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
+++ b/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Redemptions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">REPORTING PERIOD: </t>
   </si>
   <si>
-    <t>01-Jul-2023 To 22-Jun-2024</t>
+    <t>01-Jul-2023 To 24-Jun-2024</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL FACE VALUE: </t>
@@ -615,7 +615,9 @@
     <xf numFmtId="0" fontId="3" applyFont="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1"/>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="165" applyNumberFormat="1" fontId="0"/>
     <xf numFmtId="166" applyNumberFormat="1" fontId="0"/>
   </cellXfs>
@@ -661,9 +663,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.132932662963867" customWidth="1"/>
-    <col min="2" max="2" width="30.771818161010742" customWidth="1"/>
-    <col min="3" max="3" width="27.384668350219727" customWidth="1"/>
+    <col min="1" max="1" width="30.771818161010742" customWidth="1"/>
+    <col min="2" max="2" width="27.384668350219727" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="16.294299125671387" customWidth="1"/>
     <col min="5" max="5" width="12.20789623260498" customWidth="1"/>
     <col min="6" max="6" width="17.799227714538574" customWidth="1"/>
@@ -678,47 +680,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="B5" s="6">
         <v>-7208</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6">
+      <c r="B6" s="6">
         <v>-3055.28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checkin feedback changes resend email and bcc
</commit_message>
<xml_diff>
--- a/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
+++ b/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>REDEMPTIONS REPORT</t>
   </si>
@@ -20,7 +20,7 @@
     <t xml:space="preserve">STORE NAME: </t>
   </si>
   <si>
-    <t>98 | Waterlooville Golf Club- PGA Professional James Crawford</t>
+    <t>388 | Lancashire Golf Academy</t>
   </si>
   <si>
     <t xml:space="preserve">PRODUCT NAME: </t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">REPORTING PERIOD: </t>
   </si>
   <si>
-    <t>01-Jul-2024 To 07-Jul-2024</t>
+    <t>03-Jun-2024 To 09-Jun-2024</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL FACE VALUE: </t>
@@ -83,16 +83,19 @@
     <t>Statement Amt</t>
   </si>
   <si>
-    <t>Waterlooville Golf Club- PGA Pro James Crawford</t>
-  </si>
-  <si>
-    <t>PO8 8AP</t>
-  </si>
-  <si>
-    <t>EP0130108000000598</t>
-  </si>
-  <si>
-    <t>1276720122</t>
+    <t>Lancashire Golf Academy</t>
+  </si>
+  <si>
+    <t>BB1 9LF</t>
+  </si>
+  <si>
+    <t>EP0130108000000525</t>
+  </si>
+  <si>
+    <t>1241458099</t>
+  </si>
+  <si>
+    <t>GCP0000060</t>
   </si>
   <si>
     <t>Totals</t>
@@ -205,13 +208,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.771818161010742" customWidth="1"/>
-    <col min="2" max="2" width="62.246273040771484" customWidth="1"/>
+    <col min="2" max="2" width="31.101184844970703" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="16.294299125671387" customWidth="1"/>
     <col min="5" max="5" width="11.114240646362305" customWidth="1"/>
     <col min="6" max="6" width="17.799227714538574" customWidth="1"/>
     <col min="7" max="7" width="10.799415588378906" customWidth="1"/>
-    <col min="8" max="8" width="43.91780471801758" customWidth="1"/>
+    <col min="8" max="8" width="22.75058364868164" customWidth="1"/>
     <col min="9" max="9" width="11.174880027770996" customWidth="1"/>
     <col min="10" max="10" width="20.365819931030273" customWidth="1"/>
     <col min="11" max="11" width="11.634980201721191" customWidth="1"/>
@@ -254,7 +257,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>-200</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="6">
@@ -262,7 +265,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="6">
-        <v>-168.8</v>
+        <v>-63.3</v>
       </c>
     </row>
     <row r="7">
@@ -311,25 +314,25 @@
     </row>
     <row r="8">
       <c r="A8" s="7">
-        <v>45477.43819444445</v>
+        <v>45446.84405092592</v>
       </c>
       <c r="B8" s="4">
-        <v>-200</v>
+        <v>-75</v>
       </c>
       <c r="C8" s="0">
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>-26</v>
+        <v>-9.75</v>
       </c>
       <c r="E8" s="4">
-        <v>-5.2</v>
+        <v>-1.95</v>
       </c>
       <c r="F8" s="4">
-        <v>-168.8</v>
+        <v>-63.3</v>
       </c>
       <c r="G8" s="0">
-        <v>98</v>
+        <v>388</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>23</v>
@@ -343,29 +346,34 @@
       <c r="K8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="8"/>
+      <c r="L8" s="8">
+        <v>45491.647632025466</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="N8" s="4">
-        <v>0</v>
+        <v>63.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5">
-        <v>-200</v>
+        <v>-75</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>-26</v>
+        <v>-9.75</v>
       </c>
       <c r="E9" s="5">
-        <v>-5.2</v>
+        <v>-1.95</v>
       </c>
       <c r="F9" s="5">
-        <v>-168.8</v>
+        <v>-63.3</v>
       </c>
     </row>
     <row r="10"/>

</xml_diff>

<commit_message>
StoreNo changed to string datatype
</commit_message>
<xml_diff>
--- a/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
+++ b/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
@@ -7,12 +7,12 @@
   <sheets>
     <sheet name="Redemptions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1" fullPrecision="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>REDEMPTIONS REPORT</t>
   </si>
@@ -20,7 +20,7 @@
     <t xml:space="preserve">STORE NAME: </t>
   </si>
   <si>
-    <t>0 | All Stores</t>
+    <t>80 | Vale Royal Abbey Golf Club- PGA Professional Ben Derbyshire</t>
   </si>
   <si>
     <t xml:space="preserve">PRODUCT NAME: </t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">REPORTING PERIOD: </t>
   </si>
   <si>
-    <t>01-Aug-2023 To 31-Aug-2023</t>
+    <t>24-Jun-2024 To 30-Jun-2024</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL FACE VALUE: </t>
@@ -81,14 +81,37 @@
   </si>
   <si>
     <t>Statement Amt</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Vale Royal Abbey Golf Club- PGA Professional Ben Derbyshire</t>
+  </si>
+  <si>
+    <t>CW8 2BA</t>
+  </si>
+  <si>
+    <t>EP0130108000000569</t>
+  </si>
+  <si>
+    <t>1275910055</t>
+  </si>
+  <si>
+    <t>GCP64</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="£#,##0.00;[Red](£#,##0.00)"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -132,14 +155,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" applyFont="1"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="0"/>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,10 +175,33 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:N10" headerRowCount="1">
+  <autoFilter ref="A7:N10"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="TransactionDateTime"/>
+    <tableColumn id="2" name="Value"/>
+    <tableColumn id="3" name="Count"/>
+    <tableColumn id="4" name="Product Comm"/>
+    <tableColumn id="5" name="VAT Due"/>
+    <tableColumn id="6" name="Amount Payable"/>
+    <tableColumn id="7" name="Store No"/>
+    <tableColumn id="8" name="Store Name"/>
+    <tableColumn id="9" name="Postcode"/>
+    <tableColumn id="10" name="Transaction ID"/>
+    <tableColumn id="11" name="Card ID"/>
+    <tableColumn id="12" name="Statement Date"/>
+    <tableColumn id="13" name="Statement No."/>
+    <tableColumn id="14" name="Statement Amt"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" state="frozen" activePane="bottomLeft"/>
@@ -161,19 +211,19 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.771818161010742" customWidth="1"/>
-    <col min="2" max="2" width="29.069934844970703" customWidth="1"/>
+    <col min="2" max="2" width="65.4159164428711" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.044299125671387" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.549227714538574" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.296345710754395" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.606428146362305" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.861727714538574" customWidth="1"/>
-    <col min="13" max="13" width="13.758864402770996" customWidth="1"/>
-    <col min="14" max="14" width="14.412603378295898" customWidth="1"/>
+    <col min="4" max="4" width="16.294299125671387" customWidth="1"/>
+    <col min="5" max="5" width="11.114240646362305" customWidth="1"/>
+    <col min="6" max="6" width="17.799227714538574" customWidth="1"/>
+    <col min="7" max="7" width="10.799415588378906" customWidth="1"/>
+    <col min="8" max="8" width="54.43082046508789" customWidth="1"/>
+    <col min="9" max="9" width="11.174880027770996" customWidth="1"/>
+    <col min="10" max="10" width="20.365819931030273" customWidth="1"/>
+    <col min="11" max="11" width="11.634980201721191" customWidth="1"/>
+    <col min="12" max="12" width="17.111727714538574" customWidth="1"/>
+    <col min="13" max="13" width="16.008864402770996" customWidth="1"/>
+    <col min="14" max="14" width="16.6626033782959" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -209,16 +259,16 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
+      <c r="B5" s="6">
+        <v>-100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
+      <c r="B6" s="6">
+        <v>-84.4</v>
       </c>
     </row>
     <row r="7">
@@ -265,7 +315,75 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="7">
+        <v>45468.390810185185</v>
+      </c>
+      <c r="B8" s="4">
+        <v>-100</v>
+      </c>
+      <c r="C8" s="0">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>-13</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-2.6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>-84.4</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="8">
+        <v>45692.51587704861</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="4">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-100</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-13</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-2.6</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-84.4</v>
+      </c>
+    </row>
+    <row r="10"/>
   </sheetData>
   <headerFooter/>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stop zero payable remiitance
</commit_message>
<xml_diff>
--- a/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
+++ b/EPAYGOLF/wwwroot/Document/RedemptionsReporting.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>REDEMPTIONS REPORT</t>
   </si>
@@ -20,7 +20,7 @@
     <t xml:space="preserve">STORE NAME: </t>
   </si>
   <si>
-    <t>191 | Rochdale Golf Club- PGA Professional Andrew Laverty</t>
+    <t>261 | Bondhay Golf Club</t>
   </si>
   <si>
     <t xml:space="preserve">PRODUCT NAME: </t>
@@ -83,37 +83,22 @@
     <t>Statement Amt</t>
   </si>
   <si>
-    <t>191</t>
-  </si>
-  <si>
-    <t>Rochdale Golf Club- PGA Professional Andrew Laverty</t>
-  </si>
-  <si>
-    <t>OL11 5YR</t>
-  </si>
-  <si>
-    <t>EP0130108000003141</t>
-  </si>
-  <si>
-    <t>1525200785</t>
-  </si>
-  <si>
-    <t>EP0130108000003126</t>
-  </si>
-  <si>
-    <t>1525200784</t>
-  </si>
-  <si>
-    <t>EP0130108000003122</t>
-  </si>
-  <si>
-    <t>1525200786</t>
-  </si>
-  <si>
-    <t>EP0130108000003118</t>
-  </si>
-  <si>
-    <t>1525200787</t>
+    <t>261</t>
+  </si>
+  <si>
+    <t>Bondhay Golf Club</t>
+  </si>
+  <si>
+    <t>S80 3EH</t>
+  </si>
+  <si>
+    <t>EP0130108000003184</t>
+  </si>
+  <si>
+    <t>1295188330</t>
+  </si>
+  <si>
+    <t>GCP0000273</t>
   </si>
   <si>
     <t>Totals</t>
@@ -191,8 +176,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:N13" headerRowCount="1">
-  <autoFilter ref="A7:N13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:N10" headerRowCount="1">
+  <autoFilter ref="A7:N10"/>
   <tableColumns count="14">
     <tableColumn id="1" name="TransactionDateTime"/>
     <tableColumn id="2" name="Value"/>
@@ -216,7 +201,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" state="frozen" activePane="bottomLeft"/>
@@ -226,13 +211,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.771818161010742" customWidth="1"/>
-    <col min="2" max="2" width="59.0543098449707" customWidth="1"/>
+    <col min="2" max="2" width="26.699399948120117" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="16.294299125671387" customWidth="1"/>
-    <col min="5" max="5" width="10.69301700592041" customWidth="1"/>
+    <col min="5" max="5" width="11.114240646362305" customWidth="1"/>
     <col min="6" max="6" width="17.799227714538574" customWidth="1"/>
     <col min="7" max="7" width="10.799415588378906" customWidth="1"/>
-    <col min="8" max="8" width="47.719512939453125" customWidth="1"/>
+    <col min="8" max="8" width="16.963106155395508" customWidth="1"/>
     <col min="9" max="9" width="11.174880027770996" customWidth="1"/>
     <col min="10" max="10" width="20.365819931030273" customWidth="1"/>
     <col min="11" max="11" width="11.634980201721191" customWidth="1"/>
@@ -275,7 +260,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>-500</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="6">
@@ -283,7 +268,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="6">
-        <v>0</v>
+        <v>-42.2</v>
       </c>
     </row>
     <row r="7">
@@ -332,7 +317,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7">
-        <v>45852.721550925926</v>
+        <v>45855.610972222225</v>
       </c>
       <c r="B8" s="4">
         <v>-50</v>
@@ -341,13 +326,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>-6.5</v>
       </c>
       <c r="E8" s="4">
-        <v>0</v>
+        <v>-1.3</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>-42.2</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>23</v>
@@ -364,153 +349,37 @@
       <c r="K8" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8"/>
+      <c r="L8" s="8">
+        <v>45862.51995459491</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="N8" s="4">
-        <v>0</v>
+        <v>42.2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7">
-        <v>45852.519212962965</v>
-      </c>
-      <c r="B9" s="4">
-        <v>-250</v>
-      </c>
-      <c r="C9" s="0">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-50</v>
+      </c>
+      <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9"/>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7">
-        <v>45852.51866898148</v>
-      </c>
-      <c r="B10" s="4">
-        <v>-100</v>
-      </c>
-      <c r="C10" s="0">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="8"/>
-      <c r="M10"/>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7">
-        <v>45852.517905092594</v>
-      </c>
-      <c r="B11" s="4">
-        <v>-100</v>
-      </c>
-      <c r="C11" s="0">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11" s="8"/>
-      <c r="M11"/>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="5">
-        <v>-500</v>
-      </c>
-      <c r="C12" s="1">
-        <v>4</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13"/>
+      <c r="D9" s="5">
+        <v>-6.5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-1.3</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-42.2</v>
+      </c>
+    </row>
+    <row r="10"/>
   </sheetData>
   <headerFooter/>
   <tableParts>

</xml_diff>